<commit_message>
drill down updated to check of the highest and lowest value
</commit_message>
<xml_diff>
--- a/data/describe/WVS_qualities.xlsx
+++ b/data/describe/WVS_qualities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Green_Git\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664162C3-EC94-4256-9D1A-ED556E11BCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD7170-18A3-419E-8033-1B4A45B0C982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,57 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t xml:space="preserve"> What is the primary purpose of the World Values Survey (WVS)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The WVS aims to study social, political, economic, religious, and cultural values across different countries and examine how these values influence societal development over time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Who uses the data from the World Values Survey?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Researchers, policy makers, government officials, journalists, and organizations like the World Bank use WVS data for analysis in fields such as economic development, democratization, and social capital.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What are the two major dimensions of cultural variation identified by Inglehart and Welzel in the WVS?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What do traditional values emphasize according to the WVS?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Traditional values emphasize religion, family ties, authority, and a nationalistic outlook, rejecting divorce, abortion, euthanasia, and suicide.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> How do secular-rational values differ from traditional values?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Secular-rational values place less emphasis on religion, family authority, and are more accepting of divorce, abortion, and euthanasia.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve"> What do survival values prioritize?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Survival values emphasize economic and physical security, with a focus on ethnocentrism and lower levels of trust and tolerance.</t>
   </si>
   <si>
     <t xml:space="preserve"> What are self-expression values in the context of the WVS?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Self-expression values prioritize environmental protection, tolerance of diverse groups, gender equality, and political participation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What does a high score in "Fairness" indicate?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> What does "Societal Tranquillity" measure?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Societal Tranquillity measures the level of worry people feel about societal events like war, terrorism, and employment, reflecting a sense of peace and safety.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> What factors influence a low score in Societal Tranquillity?</t>
   </si>
   <si>
     <t xml:space="preserve"> What does “Neutrality” measure in the context of the WVS?</t>
@@ -82,34 +40,58 @@
     <t xml:space="preserve"> What does the "Scepticism" value represent in the context of the WVS?</t>
   </si>
   <si>
-    <t xml:space="preserve"> What does a high "Scepticism" score indicate?</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
     <t>assistant</t>
   </si>
   <si>
-    <t>The two major dimensions of cultural variation identified by Inglehart and Welzel in the WVS are "Traditional values versus Secular-rational values" and "Survival values versus Self-expression values."</t>
+    <t>The WVS aims to study social, political, economic, religious, and cultural values across different countries and examine how these values influence societal development over time.</t>
   </si>
   <si>
-    <t>Neutrality measures a lack of engagement in civic, political, or social organizations, with high-scoring countries having little participation in such groups.</t>
+    <t>Researchers, policy makers, government officials, journalists, and organizations like the World Bank use WVS data for analysis in fields such as economic development, democratization, and social capital.</t>
   </si>
   <si>
-    <t>Fairness is measured by attitudes toward whether actions like stealing, bribery, and violence are ever justifiable, reflecting societal values around justice.</t>
+    <t>Who uses the data from the World Values Survey?</t>
   </si>
   <si>
-    <t>Scepticism represents distrust in large organizations and institutions, holding them accountable through democratic processes.</t>
+    <t>What is the primary purpose of the World Values Survey (WVS)?</t>
   </si>
   <si>
-    <t xml:space="preserve"> A high score in fairness indicates that a majority of the population believes actions like stealing and bribery are never justifiable.</t>
+    <t>What are the two major dimensions of cultural variation identified by Inglehart and Welzel in the WVS?</t>
   </si>
   <si>
-    <t xml:space="preserve"> A high score in scepticism indicates that a significant portion of the population has low confidence in major institutions such as government and corporations.</t>
+    <t>What do traditional values emphasize according to the WVS?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Low scores in tranquillity are influenced by high levels of societal anxiety about issues like war, terrorism, and economic stability.</t>
+    <t>Traditional values emphasize religion, authority, and a nationalistic outlook, while rejecting abortion.</t>
+  </si>
+  <si>
+    <t>Secular values place less emphasis on religion, authority, independence and perseverance in children and are more accepting of abortion.</t>
+  </si>
+  <si>
+    <t>How do secular values differ from traditional values?</t>
+  </si>
+  <si>
+    <t>The two major dimensions of cultural variation identified by Inglehart and Welzel in the WVS are "Traditional values versus Secular values" and "Survival values versus Self-expression values".</t>
+  </si>
+  <si>
+    <t>Survival values emphasize economic and physical security, with a focus on national identity and lower levels of trust and tolerance of homosexuality.</t>
+  </si>
+  <si>
+    <t>Self-expression values prioritize leisure over work, tolerance of homosexuality, freedom, and political participation. Levels of trust are higher as well as ratings of happiness and life-satisfaction.</t>
+  </si>
+  <si>
+    <t>Neutrality measures a lack of engagement in civic, political, or social organizations. High-scoring countries having little participation in consumer organisations, charitable or humanitarian organizations, professional organizations or self-help or mutual aid groups.</t>
+  </si>
+  <si>
+    <t>Fairness is measured by attitudes toward whether the actions of stealing, bribery, cheating on taxes, and violence are ever justifiable. A high score in fairness is associated with these actions never being justifiable.</t>
+  </si>
+  <si>
+    <t>Scepticism represents distrust in government, civil services, political parties, and the justice system or courts. A high score in scepticism indicates a low confidence in these institutions.</t>
+  </si>
+  <si>
+    <t>Societal Tranquillity measures the level of worry felt about war, civil war, terrorism, and access to good education. Low scores in societal tranquillity indicate worry about these issues.</t>
   </si>
 </sst>
 </file>
@@ -185,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -211,6 +193,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1342,10 +1327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B936"/>
+  <dimension ref="A1:B933"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1356,123 +1341,108 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="9" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="12" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="B12" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>29</v>
-      </c>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
@@ -4227,15 +4197,6 @@
     </row>
     <row r="933" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A933" s="6"/>
-    </row>
-    <row r="934" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A934" s="6"/>
-    </row>
-    <row r="935" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A935" s="6"/>
-    </row>
-    <row r="936" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A936" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Clean up of prompting and model card
</commit_message>
<xml_diff>
--- a/data/describe/WVS_qualities.xlsx
+++ b/data/describe/WVS_qualities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amy\Desktop\Green_Git\twelve-gpt-educational\data\describe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6095792-4049-4DEE-84D8-89A7D126F242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CE6839-D366-4B18-9060-399ED53FAC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve"> What do survival values prioritize?</t>
   </si>
@@ -92,6 +92,42 @@
   </si>
   <si>
     <t xml:space="preserve"> What does the "Skepticism" value represent in the context of the WVS?</t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS, which took place from 2017 to 2022, what results were found on average across the globe for the "Traditional values versus Secular values"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 7th wave of the WVS which took place from 2017 to 2022, the average score in the "Traditional values versus Secular values" was negative, indicating that on average the participants had traditional values. </t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS, what was the global average for "Survival values versus Self-expression values"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 7th wave of the WVS which took place from 2017 to 2022, the average score in the "Survival values versus Self-expression values" was zero, indicating that on average the participants were neither survival nor self-expression orientated. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 7th wave of the WVS which took place from 2017 to 2022, the average score in "Neutrality" was positive, indicating that on average the participants did not actively participate in civic, political, or social organizations. </t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS, what was the global average for "Neutrality"?</t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS, what was the global average for "Fairness"?</t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS, what was the global average for "Skepticism"?</t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS, what was the global average for "Societal Tranquillity"?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 7th wave of the WVS which took place from 2017 to 2022, the average score in "Fairness" was postive, indicating that on average the participants reported that the actions of stealing, bribery, cheating on taxes, and violence were not justifiable. </t>
+  </si>
+  <si>
+    <t>In the 7th wave of the WVS which took place from 2017 to 2022, the average score in "Skepticism" was slightly positive, indicating that on average the participants indicated some distrust in government, civil services, political parties, and the justice system or courts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the 7th wave of the WVS which took place from 2017 to 2022, the average score in "Societal Tranquillity" was slightly negative, indicating that on average the participants reported some level of worry felt about war, civil war, terrorism, and access to good education. </t>
   </si>
 </sst>
 </file>
@@ -1327,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B933"/>
+  <dimension ref="A1:B936"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.08203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1435,64 +1471,94 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
@@ -4197,6 +4263,15 @@
     </row>
     <row r="933" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A933" s="6"/>
+    </row>
+    <row r="934" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A934" s="6"/>
+    </row>
+    <row r="935" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A935" s="6"/>
+    </row>
+    <row r="936" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A936" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>